<commit_message>
feat: Implement calculations page, update contract details tests and pages, and refresh test data.
</commit_message>
<xml_diff>
--- a/test-data/loginData1.xlsx
+++ b/test-data/loginData1.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,9 +427,6 @@
       <c r="H1" t="str">
         <v>executed</v>
       </c>
-      <c r="I1" t="str">
-        <v>expectedError</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -454,7 +451,7 @@
         <v>Pass</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -480,10 +477,7 @@
         <v>Fail</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -502,14 +496,14 @@
       <c r="E4" t="b">
         <v>0</v>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
       <c r="G4" t="str">
         <v>Fail</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -535,10 +529,7 @@
         <v>Fail</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -548,6 +539,9 @@
       <c r="B6" t="str">
         <v>Negative - Empty Email</v>
       </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
       <c r="D6" t="str">
         <v>admin</v>
       </c>
@@ -561,10 +555,7 @@
         <v>Fail</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Please enter your email</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -577,6 +568,9 @@
       <c r="C7" t="str">
         <v>admin@yourstore.com</v>
       </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
@@ -587,10 +581,7 @@
         <v>Fail</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -600,6 +591,12 @@
       <c r="B8" t="str">
         <v>Negative - Both Empty</v>
       </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
@@ -610,10 +607,7 @@
         <v>Fail</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Please enter your email</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -639,7 +633,7 @@
         <v>Fail</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -665,10 +659,7 @@
         <v>Fail</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -694,7 +685,7 @@
         <v>Fail</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -720,7 +711,7 @@
         <v>Pass</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -746,7 +737,7 @@
         <v>Pass</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -772,7 +763,7 @@
         <v>Pass</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -798,7 +789,7 @@
         <v>Fail</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -824,7 +815,7 @@
         <v>Fail</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -850,7 +841,7 @@
         <v>Fail</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -876,7 +867,7 @@
         <v>Fail</v>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -902,10 +893,7 @@
         <v>Fail</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -931,10 +919,7 @@
         <v>Fail</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -960,10 +945,7 @@
         <v>Fail</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -989,7 +971,7 @@
         <v>Fail</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1015,7 +997,7 @@
         <v>Fail</v>
       </c>
       <c r="H23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1041,7 +1023,7 @@
         <v>Fail</v>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1067,10 +1049,7 @@
         <v>Fail</v>
       </c>
       <c r="H25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1096,10 +1075,7 @@
         <v>Fail</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1125,10 +1101,7 @@
         <v>Fail</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1154,10 +1127,7 @@
         <v>Fail</v>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1183,7 +1153,7 @@
         <v>Fail</v>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1209,7 +1179,7 @@
         <v>Fail</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" xml:space="preserve">
@@ -1236,7 +1206,7 @@
         <v>Fail</v>
       </c>
       <c r="H31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1262,10 +1232,7 @@
         <v>Fail</v>
       </c>
       <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" xml:space="preserve">
@@ -1292,10 +1259,7 @@
         <v>Fail</v>
       </c>
       <c r="H33" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1321,10 +1285,7 @@
         <v>Fail</v>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1350,10 +1311,7 @@
         <v>Fail</v>
       </c>
       <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1379,10 +1337,7 @@
         <v>Fail</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1408,7 +1363,7 @@
         <v>Fail</v>
       </c>
       <c r="H37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1434,7 +1389,7 @@
         <v>Fail</v>
       </c>
       <c r="H38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1460,7 +1415,7 @@
         <v>Fail</v>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1486,7 +1441,7 @@
         <v>Fail</v>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1512,10 +1467,7 @@
         <v>Fail</v>
       </c>
       <c r="H41" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1541,10 +1493,7 @@
         <v>Fail</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1570,7 +1519,7 @@
         <v>Pass</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1596,7 +1545,7 @@
         <v>Pass</v>
       </c>
       <c r="H44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1622,7 +1571,7 @@
         <v>Fail</v>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1648,7 +1597,7 @@
         <v>Fail</v>
       </c>
       <c r="H46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1674,7 +1623,7 @@
         <v>Fail</v>
       </c>
       <c r="H47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1700,7 +1649,7 @@
         <v>Fail</v>
       </c>
       <c r="H48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1726,10 +1675,7 @@
         <v>Fail</v>
       </c>
       <c r="H49" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1755,10 +1701,7 @@
         <v>Fail</v>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
-      </c>
-      <c r="I50" t="str">
-        <v>Sorry, you have been blocked</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1784,10 +1727,7 @@
         <v>Fail</v>
       </c>
       <c r="H51" t="b">
-        <v>1</v>
-      </c>
-      <c r="I51" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1813,10 +1753,7 @@
         <v>Fail</v>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
-      </c>
-      <c r="I52" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1842,7 +1779,7 @@
         <v>Fail</v>
       </c>
       <c r="H53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1868,7 +1805,7 @@
         <v>Fail</v>
       </c>
       <c r="H54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1894,7 +1831,7 @@
         <v>Fail</v>
       </c>
       <c r="H55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1920,7 +1857,7 @@
         <v>Fail</v>
       </c>
       <c r="H56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1946,15 +1883,12 @@
         <v>Fail</v>
       </c>
       <c r="H57" t="b">
-        <v>1</v>
-      </c>
-      <c r="I57" t="str">
-        <v>Login was unsuccessful</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I57"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H57"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>